<commit_message>
Add `owndat` and `asmt` fields to IC PIN-level reference file output
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_non_res_pin_level_data.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_non_res_pin_level_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10D3767-06EF-4369-8B8F-F4F424A2D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551BCBE-A01A-4853-A465-1AFFBF3C8EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>PARDAT</t>
   </si>
@@ -98,16 +98,43 @@
   </si>
   <si>
     <t>OWN1</t>
+  </si>
+  <si>
+    <t>ASMT</t>
+  </si>
+  <si>
+    <t>ADDR1</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>VALASM1</t>
+  </si>
+  <si>
+    <t>VALASM2</t>
+  </si>
+  <si>
+    <t>VALASM3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -464,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +567,29 @@
       <c r="W1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,8 +659,30 @@
       <c r="W2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="X2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add `owndat` and `asmt` fields to IC PIN-level reference file output (#841)
* Add `owndat` and `asmt` fields to IC PIN-level reference file output

* Add rolltype != 'RR' filter to IC reference PIN-level tables
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_non_res_pin_level_data.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_non_res_pin_level_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10D3767-06EF-4369-8B8F-F4F424A2D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551BCBE-A01A-4853-A465-1AFFBF3C8EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>PARDAT</t>
   </si>
@@ -98,16 +98,43 @@
   </si>
   <si>
     <t>OWN1</t>
+  </si>
+  <si>
+    <t>ASMT</t>
+  </si>
+  <si>
+    <t>ADDR1</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>VALASM1</t>
+  </si>
+  <si>
+    <t>VALASM2</t>
+  </si>
+  <si>
+    <t>VALASM3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -464,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +567,29 @@
       <c r="W1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,8 +659,30 @@
       <c r="W2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="X2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>